<commit_message>
Update ERD to Game and Time-Record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF046140-D882-44CD-BDC0-2805DD1A9A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D26DD08-5EAA-4C83-9C1C-717EC39936E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -238,6 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -920,7 +921,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,8 +1433,8 @@
         <v>25</v>
       </c>
       <c r="C54" s="12">
-        <f>38/60</f>
-        <v>0.6333333333333333</v>
+        <f>57/60</f>
+        <v>0.95</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>4</v>
@@ -1485,15 +1486,15 @@
       </c>
       <c r="B62" s="13">
         <f>C50+C51+C54+C46+C47</f>
-        <v>4.83</v>
+        <v>5.1466666666666665</v>
       </c>
       <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
-      <c r="B63" s="4">
+      <c r="B63" s="14">
         <f>B60+B61+B62</f>
-        <v>4.83</v>
+        <v>5.1466666666666665</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="6"/>

</xml_diff>

<commit_message>
Add ERD and update time record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D26DD08-5EAA-4C83-9C1C-717EC39936E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FD151F-0623-4FEE-82B4-3DF5CB6DDDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
@@ -105,13 +105,13 @@
     <t>Wrote ReadMe file</t>
   </si>
   <si>
-    <t>Creating ERD</t>
-  </si>
-  <si>
     <t>Editing ERD</t>
   </si>
   <si>
     <t>Adding new Tables to ERD</t>
+  </si>
+  <si>
+    <t>Creating first version of ERD</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1371,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C47">
         <v>1.5</v>
@@ -1393,7 +1393,7 @@
         <v>44571</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50">
         <v>1.33</v>
@@ -1407,7 +1407,7 @@
         <v>44574</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C51" s="12">
         <f>40/60</f>
@@ -1430,11 +1430,11 @@
         <v>44577</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C54" s="12">
-        <f>57/60</f>
-        <v>0.95</v>
+        <f>86/60</f>
+        <v>1.4333333333333333</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>4</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B62" s="13">
         <f>C50+C51+C54+C46+C47</f>
-        <v>5.1466666666666665</v>
+        <v>5.63</v>
       </c>
       <c r="D62" s="5"/>
     </row>
@@ -1494,7 +1494,7 @@
       <c r="A63" s="4"/>
       <c r="B63" s="14">
         <f>B60+B61+B62</f>
-        <v>5.1466666666666665</v>
+        <v>5.63</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="6"/>

</xml_diff>

<commit_message>
Update ERD and Time-Record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62030BDD-4D0F-4BB0-822C-582C69938C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BBF81D-AF5D-4A24-8E53-3164FA3CAAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Creating final ERD</t>
+  </si>
+  <si>
+    <t>Help to edit website</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3547AEA-3C2E-4B53-BBD6-378E3F7BB292}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,7 +1767,7 @@
         <v>34</v>
       </c>
       <c r="C83" s="12">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>3</v>
@@ -1772,8 +1775,15 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="5"/>
+      <c r="B84" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="12">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D85" s="5"/>
@@ -1812,8 +1822,8 @@
         <v>3</v>
       </c>
       <c r="B91" s="13">
-        <f>C75+C76+C79+C80+C81+C83</f>
-        <v>11</v>
+        <f>C75+C76+C79+C80+C81+C83+C84</f>
+        <v>11.67</v>
       </c>
       <c r="D91" s="5"/>
     </row>
@@ -1821,7 +1831,7 @@
       <c r="A92" s="4"/>
       <c r="B92" s="14">
         <f>B89+B90+B91</f>
-        <v>11</v>
+        <v>11.67</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="6"/>

</xml_diff>

<commit_message>
Update ERD and Time record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phili\Documents\GitHub\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174105F9-2409-478B-88D2-1A08CD35A42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9607A60A-F767-4CEA-AF07-A21FB56DB4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1829,39 +1829,39 @@
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C86" s="12">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
+      <c r="A87" s="1">
+        <v>44591</v>
+      </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C87" s="12">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="D87" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="12">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
-        <v>44591</v>
-      </c>
-      <c r="B88" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" s="12">
-        <v>1.33</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1915,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="B94" s="12">
-        <f>C76+C79+C86+C87+C89</f>
+        <f>C76+C79+C86+C88+C89</f>
         <v>11.5</v>
       </c>
       <c r="D94" s="5"/>
@@ -1935,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B96" s="13">
-        <f>C91+C88+C83+C82+C81+C80+C77</f>
+        <f>C91+C87+C83+C82+C81+C80+C77</f>
         <v>13</v>
       </c>
       <c r="D96" s="5"/>

</xml_diff>

<commit_message>
Update Time-Record and add ERD for website
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phili\Documents\GitHub\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC309F0-21BD-4175-8538-C524A4E198CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76179A2-3B2D-4ACF-B069-C72CE02CC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -712,6 +712,66 @@
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:t>Sprint 4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3223260" cy="512769"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Textfeld 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF729FA1-1C24-4BBB-8C66-A60C5E5A8297}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12778740"/>
+          <a:ext cx="3223260" cy="512769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-AT" sz="2800" b="1">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Sprint 5</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1018,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3547AEA-3C2E-4B53-BBD6-378E3F7BB292}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,6 +2054,142 @@
       <c r="C100" s="4"/>
       <c r="D100" s="6"/>
     </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="15"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="5"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="5"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" s="12"/>
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" s="12"/>
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" s="13"/>
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="4"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Update time record and game
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DFF3C9-2981-4908-B87B-CC577F33F748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF78B893-1AE0-4663-989A-B0650C3F01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Teamtalk about next targets</t>
+  </si>
+  <si>
+    <t>Adding a new puzlle and editing enviroment</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1093,7 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2164,9 +2167,18 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1"/>
-      <c r="C114" s="12"/>
-      <c r="D114" s="15"/>
+      <c r="A114" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B114" t="s">
+        <v>42</v>
+      </c>
+      <c r="C114" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
@@ -2228,7 +2240,8 @@
         <v>3</v>
       </c>
       <c r="B125" s="13">
-        <v>4.58</v>
+        <f>C110+C109+C112+C114</f>
+        <v>7.0830000000000002</v>
       </c>
       <c r="D125" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update Game and Time record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phili\Documents\GitHub\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECDAD48-DD1D-4FDD-8832-7D1E6D518B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711417DC-8792-493D-B3A6-2A4242B237FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Tried to implement custom controls</t>
+  </si>
+  <si>
+    <t>Adding new puzzle</t>
+  </si>
+  <si>
+    <t>Fixing buggs of new puzzle</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3547AEA-3C2E-4B53-BBD6-378E3F7BB292}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,14 +2288,32 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
-      <c r="C122" s="12"/>
-      <c r="D122" s="5"/>
+      <c r="A122" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B122" t="s">
+        <v>47</v>
+      </c>
+      <c r="C122" s="12">
+        <v>4</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="5"/>
+      <c r="A123" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C123" s="12">
+        <v>2</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
@@ -2332,17 +2356,18 @@
         <v>3</v>
       </c>
       <c r="B129" s="13">
-        <v>7.58</v>
-      </c>
+        <v>13.58</v>
+      </c>
+      <c r="C129" s="12"/>
       <c r="D129" s="5"/>
     </row>
-    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="4"/>
       <c r="B130" s="14">
         <f>B129+B128+B127</f>
-        <v>23.08</v>
-      </c>
-      <c r="C130" s="13"/>
+        <v>29.08</v>
+      </c>
+      <c r="C130" s="14"/>
       <c r="D130" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update game, erd and time-record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711417DC-8792-493D-B3A6-2A4242B237FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE8A529-8D39-4011-8EC4-EB8445C02CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Fixing buggs of new puzzle</t>
+  </si>
+  <si>
+    <t>Editing puzzles, enviroment and erd</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3547AEA-3C2E-4B53-BBD6-378E3F7BB292}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2316,8 +2319,18 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="1"/>
-      <c r="D124" s="5"/>
+      <c r="A124" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B124" t="s">
+        <v>49</v>
+      </c>
+      <c r="C124" s="12">
+        <v>1.42</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D125" s="5"/>
@@ -2356,7 +2369,7 @@
         <v>3</v>
       </c>
       <c r="B129" s="13">
-        <v>13.58</v>
+        <v>15</v>
       </c>
       <c r="C129" s="12"/>
       <c r="D129" s="5"/>
@@ -2365,7 +2378,7 @@
       <c r="A130" s="4"/>
       <c r="B130" s="14">
         <f>B129+B128+B127</f>
-        <v>29.08</v>
+        <v>30.5</v>
       </c>
       <c r="C130" s="14"/>
       <c r="D130" s="6"/>

</xml_diff>

<commit_message>
Update Game and Time-Record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF0EDDF-FCF7-4A26-93AB-97A1A4513E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F4082E-C617-43DF-BBED-A84F3F5B06AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4E1D2B5-DAF4-440D-A6A9-5B95092B556F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Working on Quarkus application</t>
+  </si>
+  <si>
+    <t>Watching blender tutorials and creating first model</t>
+  </si>
+  <si>
+    <t>Finishing first model and implementing it into unity</t>
   </si>
 </sst>
 </file>
@@ -897,6 +903,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3223260" cy="512769"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Textfeld 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC8619C-1FFF-4BFB-9CA6-8E3ED873F215}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="26117550"/>
+          <a:ext cx="3223260" cy="512769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-AT" sz="2800" b="1">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Sprint 7</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1197,16 +1263,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3547AEA-3C2E-4B53-BBD6-378E3F7BB292}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G196" sqref="G196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
@@ -2824,6 +2890,189 @@
       <c r="C168" s="14"/>
       <c r="D168" s="6"/>
     </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3"/>
+      <c r="C175" s="16"/>
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="16"/>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3"/>
+      <c r="C177" s="16"/>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C179" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D179" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="1"/>
+      <c r="D180" s="5"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="1"/>
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="1"/>
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B183" t="s">
+        <v>58</v>
+      </c>
+      <c r="C183" s="12">
+        <v>5</v>
+      </c>
+      <c r="D183" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="1"/>
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="1"/>
+      <c r="D185" s="5"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="1"/>
+      <c r="D186" s="15"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="1"/>
+      <c r="D187" s="15"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" s="1"/>
+      <c r="D188" s="15"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="1">
+        <v>44647</v>
+      </c>
+      <c r="B189" t="s">
+        <v>59</v>
+      </c>
+      <c r="C189" s="12">
+        <v>3</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="1"/>
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="1"/>
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="1"/>
+      <c r="D192" s="5"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="1"/>
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="1"/>
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="1"/>
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="1"/>
+      <c r="D196" s="5"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" s="1"/>
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" s="1"/>
+      <c r="D198" s="5"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" s="1"/>
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="1"/>
+      <c r="D200" s="5"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D201" s="5"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>5</v>
+      </c>
+      <c r="B202" s="12"/>
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>7</v>
+      </c>
+      <c r="B203" s="12"/>
+      <c r="D203" s="5"/>
+    </row>
+    <row r="204" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" s="13">
+        <v>8</v>
+      </c>
+      <c r="D204" s="5"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="4"/>
+      <c r="B205" s="14">
+        <f>SUM(B202:B204)</f>
+        <v>8</v>
+      </c>
+      <c r="C205" s="14"/>
+      <c r="D205" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding first part of labirinth
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\HTL\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD4B4C6-656D-4820-911C-AA6941AD3C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E6FF85-937E-4038-8CD8-8A281A361E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="3300" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -239,6 +239,21 @@
   </si>
   <si>
     <t>Working on multiplayer</t>
+  </si>
+  <si>
+    <t>Watching Blender tutorials and creating models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating first puzzle model </t>
+  </si>
+  <si>
+    <t>Fixing model for first puzzle</t>
+  </si>
+  <si>
+    <t>Editing scaling of player and eviroment</t>
+  </si>
+  <si>
+    <t>Fixing labirinth model</t>
   </si>
 </sst>
 </file>
@@ -1349,45 +1364,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D235" sqref="D235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="16"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="16"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="16"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="16"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44534</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44535</v>
       </c>
@@ -1429,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1441,7 +1456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44536</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -1467,12 +1482,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1496,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1491,7 +1506,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1516,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1511,7 +1526,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="10">
         <f>B13+B14+B15</f>
@@ -1520,43 +1535,43 @@
       <c r="C16" s="14"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44543</v>
       </c>
@@ -1584,7 +1599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>10</v>
@@ -1596,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>11</v>
@@ -1608,7 +1623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44545</v>
       </c>
@@ -1622,7 +1637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>13</v>
@@ -1634,7 +1649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>14</v>
@@ -1646,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44549</v>
       </c>
@@ -1660,7 +1675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
         <v>16</v>
@@ -1672,7 +1687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>17</v>
@@ -1684,10 +1699,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>1</v>
       </c>
@@ -1696,7 +1711,7 @@
       </c>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1706,7 +1721,7 @@
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1716,7 +1731,7 @@
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1741,7 @@
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4">
         <f>B35+B36+B37</f>
@@ -1735,43 +1750,43 @@
       <c r="C38" s="14"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="16"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="16"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="16"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="16"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="16"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="16"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44550</v>
       </c>
@@ -1799,7 +1814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" t="s">
         <v>24</v>
@@ -1811,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" t="s">
         <v>26</v>
@@ -1823,7 +1838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44206</v>
       </c>
@@ -1837,7 +1852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" t="s">
         <v>22</v>
@@ -1849,7 +1864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
         <v>27</v>
@@ -1861,7 +1876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>44573</v>
       </c>
@@ -1876,7 +1891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" t="s">
         <v>27</v>
@@ -1888,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>44577</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
         <v>28</v>
@@ -1915,7 +1930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" t="s">
         <v>25</v>
@@ -1927,14 +1942,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +1958,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1953,7 +1968,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1963,7 +1978,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1973,7 +1988,7 @@
       </c>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="14">
         <f>B60+B61+B62</f>
@@ -1982,31 +1997,31 @@
       <c r="C63" s="14"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="16"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="16"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="16"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="16"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>0</v>
       </c>
@@ -2020,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>44583</v>
       </c>
@@ -2034,7 +2049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>44584</v>
       </c>
@@ -2048,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>44585</v>
       </c>
@@ -2062,7 +2077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>30</v>
       </c>
@@ -2073,7 +2088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>30</v>
       </c>
@@ -2084,7 +2099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>44587</v>
       </c>
@@ -2098,7 +2113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>44589</v>
       </c>
@@ -2112,7 +2127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>44590</v>
       </c>
@@ -2126,7 +2141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" t="s">
         <v>22</v>
@@ -2138,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" t="s">
         <v>33</v>
@@ -2150,7 +2165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" t="s">
         <v>36</v>
@@ -2162,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" t="s">
         <v>37</v>
@@ -2174,7 +2189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" t="s">
         <v>37</v>
@@ -2186,7 +2201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>44591</v>
       </c>
@@ -2200,7 +2215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" t="s">
         <v>22</v>
@@ -2212,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" t="s">
         <v>37</v>
@@ -2224,7 +2239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>37</v>
       </c>
@@ -2235,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>37</v>
       </c>
@@ -2246,7 +2261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>44592</v>
       </c>
@@ -2260,7 +2275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>44593</v>
       </c>
@@ -2274,10 +2289,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D95" s="5"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>1</v>
       </c>
@@ -2286,7 +2301,7 @@
       </c>
       <c r="D96" s="5"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -2296,7 +2311,7 @@
       </c>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2321,7 @@
       </c>
       <c r="D98" s="5"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -2316,7 +2331,7 @@
       </c>
       <c r="D99" s="5"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="14">
         <f>B99+B98+B97</f>
@@ -2325,31 +2340,31 @@
       <c r="C100" s="14"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="16"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="16"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="16"/>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="16"/>
       <c r="D106" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>44599</v>
       </c>
@@ -2377,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" t="s">
         <v>42</v>
@@ -2389,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" t="s">
         <v>40</v>
@@ -2401,7 +2416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" t="s">
         <v>40</v>
@@ -2413,7 +2428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
         <v>40</v>
@@ -2425,7 +2440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>44</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>44601</v>
       </c>
@@ -2450,7 +2465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" t="s">
         <v>46</v>
@@ -2462,7 +2477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>44603</v>
       </c>
@@ -2476,7 +2491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>44604</v>
       </c>
@@ -2490,7 +2505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>44605</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" t="s">
         <v>43</v>
@@ -2516,7 +2531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" t="s">
         <v>44</v>
@@ -2528,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>44613</v>
       </c>
@@ -2542,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>44617</v>
       </c>
@@ -2556,7 +2571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>44618</v>
       </c>
@@ -2570,7 +2585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>44619</v>
       </c>
@@ -2584,10 +2599,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D126" s="5"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2611,7 @@
       </c>
       <c r="D127" s="5"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -2606,7 +2621,7 @@
       </c>
       <c r="D128" s="5"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>7</v>
       </c>
@@ -2616,7 +2631,7 @@
       </c>
       <c r="D129" s="5"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -2625,7 +2640,7 @@
       </c>
       <c r="D130" s="5"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="4"/>
       <c r="B131" s="14">
         <f>B130+B129+B128</f>
@@ -2634,31 +2649,31 @@
       <c r="C131" s="14"/>
       <c r="D131" s="6"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="16"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="16"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="16"/>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="16"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>0</v>
       </c>
@@ -2672,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>44620</v>
       </c>
@@ -2686,7 +2701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" t="s">
         <v>51</v>
@@ -2698,7 +2713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" t="s">
         <v>51</v>
@@ -2710,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>44622</v>
       </c>
@@ -2724,7 +2739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" t="s">
         <v>52</v>
@@ -2736,7 +2751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" t="s">
         <v>52</v>
@@ -2748,7 +2763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>44626</v>
       </c>
@@ -2762,7 +2777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>44627</v>
       </c>
@@ -2776,7 +2791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" t="s">
         <v>53</v>
@@ -2788,7 +2803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" t="s">
         <v>53</v>
@@ -2800,7 +2815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" t="s">
         <v>53</v>
@@ -2812,7 +2827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>44629</v>
       </c>
@@ -2826,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" t="s">
         <v>52</v>
@@ -2838,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" t="s">
         <v>52</v>
@@ -2850,7 +2865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>44604</v>
       </c>
@@ -2864,7 +2879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
       <c r="B158" t="s">
         <v>55</v>
@@ -2876,7 +2891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1"/>
       <c r="B159" t="s">
         <v>55</v>
@@ -2888,7 +2903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>44633</v>
       </c>
@@ -2902,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" t="s">
         <v>56</v>
@@ -2914,7 +2929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" t="s">
         <v>56</v>
@@ -2926,11 +2941,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="D163" s="5"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="9" t="s">
         <v>1</v>
       </c>
@@ -2939,7 +2954,7 @@
       </c>
       <c r="D164" s="5"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>5</v>
       </c>
@@ -2948,7 +2963,7 @@
       </c>
       <c r="D165" s="5"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>7</v>
       </c>
@@ -2958,7 +2973,7 @@
       </c>
       <c r="D166" s="5"/>
     </row>
-    <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>3</v>
       </c>
@@ -2967,7 +2982,7 @@
       </c>
       <c r="D167" s="5"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="4"/>
       <c r="B168" s="14">
         <f>SUM(B165:B167)</f>
@@ -2976,31 +2991,31 @@
       <c r="C168" s="14"/>
       <c r="D168" s="6"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="16"/>
       <c r="D175" s="3"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="16"/>
       <c r="D176" s="3"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="16"/>
       <c r="D177" s="3"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="16"/>
       <c r="D178" s="3"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>0</v>
       </c>
@@ -3014,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>44634</v>
       </c>
@@ -3028,7 +3043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
       <c r="B181" t="s">
         <v>60</v>
@@ -3040,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>60</v>
       </c>
@@ -3051,7 +3066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>44636</v>
       </c>
@@ -3065,7 +3080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
         <v>63</v>
       </c>
@@ -3076,7 +3091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>44641</v>
       </c>
@@ -3090,7 +3105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
       <c r="B186" t="s">
         <v>60</v>
@@ -3102,7 +3117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
       <c r="B187" t="s">
         <v>60</v>
@@ -3114,7 +3129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>44647</v>
       </c>
@@ -3128,7 +3143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
       <c r="B189" t="s">
         <v>59</v>
@@ -3140,7 +3155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" t="s">
         <v>61</v>
@@ -3152,7 +3167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
       <c r="B191" t="s">
         <v>61</v>
@@ -3164,7 +3179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
       <c r="B192" t="s">
         <v>61</v>
@@ -3176,35 +3191,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="9" t="s">
         <v>1</v>
       </c>
@@ -3213,7 +3228,7 @@
       </c>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>5</v>
       </c>
@@ -3223,7 +3238,7 @@
       </c>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>7</v>
       </c>
@@ -3233,7 +3248,7 @@
       </c>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>3</v>
       </c>
@@ -3243,7 +3258,7 @@
       </c>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="4"/>
       <c r="B205" s="14">
         <f>SUM(B202:B204)</f>
@@ -3252,31 +3267,31 @@
       <c r="C205" s="14"/>
       <c r="D205" s="6"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
       <c r="C211" s="16"/>
       <c r="D211" s="3"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="3"/>
       <c r="B212" s="3"/>
       <c r="C212" s="16"/>
       <c r="D212" s="3"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="3"/>
       <c r="B213" s="3"/>
       <c r="C213" s="16"/>
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="16"/>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>44648</v>
       </c>
@@ -3304,14 +3319,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1"/>
-      <c r="D217" s="5"/>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>68</v>
+      </c>
+      <c r="C217" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="D217" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D218" s="5"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>44655</v>
       </c>
@@ -3325,14 +3348,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D220" s="5"/>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B220" t="s">
+        <v>69</v>
+      </c>
+      <c r="C220" s="12">
+        <v>3</v>
+      </c>
+      <c r="D220" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1"/>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>44663</v>
       </c>
@@ -3346,132 +3377,164 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
+        <v>44667</v>
+      </c>
+      <c r="B223" t="s">
+        <v>70</v>
+      </c>
+      <c r="C223" s="12">
+        <v>2</v>
+      </c>
+      <c r="D223" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="1">
         <v>44669</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B224" t="s">
         <v>66</v>
       </c>
-      <c r="C223" s="12">
+      <c r="C224" s="12">
         <v>6</v>
       </c>
-      <c r="D223" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+      <c r="D224" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="1">
         <v>44671</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B225" t="s">
         <v>67</v>
       </c>
-      <c r="C224" s="12">
+      <c r="C225" s="12">
         <v>1</v>
       </c>
-      <c r="D224" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="1"/>
-      <c r="D225" s="5"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1"/>
-      <c r="D226" s="5"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
+      <c r="B226" t="s">
+        <v>71</v>
+      </c>
+      <c r="C226" s="12">
+        <v>1</v>
+      </c>
+      <c r="D226" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="1"/>
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="1">
         <v>44674</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B228" t="s">
         <v>67</v>
       </c>
-      <c r="C227" s="12">
+      <c r="C228" s="12">
         <v>2</v>
       </c>
-      <c r="D227" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="1"/>
-      <c r="D228" s="5"/>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D229" s="5"/>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="1"/>
+      <c r="D228" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="1"/>
+      <c r="B229" t="s">
+        <v>72</v>
+      </c>
+      <c r="C229" s="12">
+        <v>2</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D230" s="5"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1"/>
       <c r="D231" s="5"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1"/>
       <c r="D232" s="5"/>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
       <c r="D233" s="5"/>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1"/>
       <c r="D234" s="5"/>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1"/>
       <c r="D235" s="5"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="1"/>
       <c r="D236" s="5"/>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="9" t="s">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="1"/>
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B237" s="9" t="s">
+      <c r="B238" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D237" s="5"/>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>5</v>
-      </c>
-      <c r="B238" s="12">
-        <f>C216+C219+C222+C223+C224+C227</f>
+      <c r="D238" s="5"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>5</v>
+      </c>
+      <c r="B239" s="12">
+        <f>C216+C219+C222+C224+C225+C228</f>
         <v>14.5</v>
       </c>
-      <c r="D238" s="5"/>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>7</v>
-      </c>
-      <c r="B239" s="12"/>
       <c r="D239" s="5"/>
     </row>
-    <row r="240" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>3</v>
-      </c>
-      <c r="B240" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="B240" s="12"/>
       <c r="D240" s="5"/>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="4"/>
-      <c r="B241" s="14">
-        <f>SUM(B238:B240)</f>
-        <v>14.5</v>
-      </c>
-      <c r="C241" s="14"/>
-      <c r="D241" s="6"/>
+    <row r="241" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>3</v>
+      </c>
+      <c r="B241" s="13">
+        <v>10.5</v>
+      </c>
+      <c r="D241" s="5"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" s="4"/>
+      <c r="B242" s="14">
+        <f>SUM(B239:B241)</f>
+        <v>25</v>
+      </c>
+      <c r="C242" s="14"/>
+      <c r="D242" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying to optimize game performence
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\HTL\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06B317B-5438-44D5-840C-6722A6839115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38A2BC-628C-4D18-AFE1-9701878BC20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Adding second part of first puzlle</t>
+  </si>
+  <si>
+    <t>Trying to optimize game performence</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3480,7 +3483,15 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1"/>
-      <c r="D231" s="5"/>
+      <c r="B231" t="s">
+        <v>74</v>
+      </c>
+      <c r="C231" s="12">
+        <v>2</v>
+      </c>
+      <c r="D231" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1"/>
@@ -3537,8 +3548,8 @@
         <v>3</v>
       </c>
       <c r="B241" s="13">
-        <f>C217+C220+C223+C226+C229+C230</f>
-        <v>15</v>
+        <f>C217+C220+C223+C226+C229+C230+C231</f>
+        <v>17</v>
       </c>
       <c r="D241" s="5"/>
     </row>
@@ -3546,7 +3557,7 @@
       <c r="A242" s="4"/>
       <c r="B242" s="14">
         <f>SUM(B239:B241)</f>
-        <v>29.5</v>
+        <v>31.5</v>
       </c>
       <c r="C242" s="14"/>
       <c r="D242" s="6"/>

</xml_diff>

<commit_message>
Update #8 and  #6
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\HTL\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A110A607-4252-41A6-A00F-4A6917682CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B82EF79-430B-4339-BF72-3E46B66EEAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Trying to fix git problems</t>
+  </si>
+  <si>
+    <t>Cleaning up reposetory</t>
+  </si>
+  <si>
+    <t>Creating a ReadMe for the different directories</t>
   </si>
 </sst>
 </file>
@@ -1103,6 +1109,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3223260" cy="512769"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Textfeld 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07D28A2-199C-485D-993C-93A393E06BF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="32450314"/>
+          <a:ext cx="3223260" cy="512769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-AT" sz="2800" b="1">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Sprint 9</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1403,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D249"/>
+  <dimension ref="A1:D285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G238" sqref="G238"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B285" sqref="B285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,6 +3796,223 @@
       <c r="C249" s="14"/>
       <c r="D249" s="6"/>
     </row>
+    <row r="254" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C254" s="21"/>
+    </row>
+    <row r="255" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="3"/>
+      <c r="B255" s="3"/>
+      <c r="C255" s="16"/>
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="3"/>
+      <c r="B256" s="3"/>
+      <c r="C256" s="16"/>
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="3"/>
+      <c r="B257" s="3"/>
+      <c r="C257" s="16"/>
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="3"/>
+      <c r="B258" s="3"/>
+      <c r="C258" s="16"/>
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C259" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D259" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="1">
+        <v>44676</v>
+      </c>
+      <c r="B260" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C260" s="21">
+        <v>2</v>
+      </c>
+      <c r="D260" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="1"/>
+      <c r="D261" s="20"/>
+    </row>
+    <row r="262" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="1">
+        <v>44678</v>
+      </c>
+      <c r="B262" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C262" s="21">
+        <v>0.67</v>
+      </c>
+      <c r="D262" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="1"/>
+      <c r="C263" s="21"/>
+      <c r="D263" s="20"/>
+    </row>
+    <row r="264" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A264" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B264" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C264" s="21">
+        <v>0.84</v>
+      </c>
+      <c r="D264" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A265" s="1"/>
+      <c r="C265" s="21"/>
+      <c r="D265" s="20"/>
+    </row>
+    <row r="266" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="1"/>
+      <c r="C266" s="21"/>
+      <c r="D266" s="20"/>
+    </row>
+    <row r="267" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="1"/>
+      <c r="C267" s="21"/>
+      <c r="D267" s="20"/>
+    </row>
+    <row r="268" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="1"/>
+      <c r="C268" s="21"/>
+      <c r="D268" s="20"/>
+    </row>
+    <row r="269" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="1"/>
+      <c r="C269" s="21"/>
+      <c r="D269" s="20"/>
+    </row>
+    <row r="270" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A270" s="1"/>
+      <c r="C270" s="21"/>
+      <c r="D270" s="20"/>
+    </row>
+    <row r="271" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A271" s="1"/>
+      <c r="C271" s="21"/>
+      <c r="D271" s="20"/>
+    </row>
+    <row r="272" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="1"/>
+      <c r="C272" s="21"/>
+      <c r="D272" s="20"/>
+    </row>
+    <row r="273" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C273" s="21"/>
+      <c r="D273" s="20"/>
+    </row>
+    <row r="274" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A274" s="1"/>
+      <c r="C274" s="21"/>
+      <c r="D274" s="20"/>
+    </row>
+    <row r="275" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="1"/>
+      <c r="C275" s="21"/>
+      <c r="D275" s="20"/>
+    </row>
+    <row r="276" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A276" s="1"/>
+      <c r="C276" s="21"/>
+      <c r="D276" s="20"/>
+    </row>
+    <row r="277" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A277" s="1"/>
+      <c r="C277" s="21"/>
+      <c r="D277" s="20"/>
+    </row>
+    <row r="278" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A278" s="1"/>
+      <c r="C278" s="21"/>
+      <c r="D278" s="20"/>
+    </row>
+    <row r="279" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A279" s="1"/>
+      <c r="C279" s="21"/>
+      <c r="D279" s="20"/>
+    </row>
+    <row r="280" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A280" s="1"/>
+      <c r="C280" s="21"/>
+      <c r="D280" s="20"/>
+    </row>
+    <row r="281" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A281" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B281" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C281" s="21"/>
+      <c r="D281" s="20"/>
+    </row>
+    <row r="282" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A282" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B282" s="21"/>
+      <c r="C282" s="21"/>
+      <c r="D282" s="20"/>
+    </row>
+    <row r="283" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A283" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B283" s="21"/>
+      <c r="C283" s="21"/>
+      <c r="D283" s="20"/>
+    </row>
+    <row r="284" spans="1:4" s="19" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A284" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B284" s="13">
+        <f>C260+C262+C264</f>
+        <v>3.51</v>
+      </c>
+      <c r="C284" s="21"/>
+      <c r="D284" s="20"/>
+    </row>
+    <row r="285" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="4"/>
+      <c r="B285" s="14">
+        <f>SUM(B282:B284)</f>
+        <v>3.51</v>
+      </c>
+      <c r="C285" s="14"/>
+      <c r="D285" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Update #6 and #8
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\Desktop\HTL\SYP\Youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B82EF79-430B-4339-BF72-3E46B66EEAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EDC38B-1ED2-49EF-89A2-8D1C89394CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>Cleaning up reposetory</t>
-  </si>
-  <si>
-    <t>Creating a ReadMe for the different directories</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B285" sqref="B285"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A265" sqref="A265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3879,10 +3876,10 @@
         <v>44689</v>
       </c>
       <c r="B264" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C264" s="21">
-        <v>0.84</v>
+        <v>1.5</v>
       </c>
       <c r="D264" s="15" t="s">
         <v>3</v>
@@ -3999,7 +3996,7 @@
       </c>
       <c r="B284" s="13">
         <f>C260+C262+C264</f>
-        <v>3.51</v>
+        <v>4.17</v>
       </c>
       <c r="C284" s="21"/>
       <c r="D284" s="20"/>
@@ -4008,7 +4005,7 @@
       <c r="A285" s="4"/>
       <c r="B285" s="14">
         <f>SUM(B282:B284)</f>
-        <v>3.51</v>
+        <v>4.17</v>
       </c>
       <c r="C285" s="14"/>
       <c r="D285" s="6"/>

</xml_diff>

<commit_message>
fix typo in time record
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJ2122\Syp\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434CF3D3-2FE2-4372-A05D-CE8C1E5B9917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0FDB3-E796-4C03-9CD8-47D7670537A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,7 @@
     <t>Fixing git problems</t>
   </si>
   <si>
-    <t>Tried to implement animations</t>
+    <t>Trying to implement animations</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1197,7 +1197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1495,11 +1495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E269" sqref="E269"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="58.44140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
add character animation to blender model
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\youre-not-alone\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amels\OneDrive\Desktop\HTL\SYP\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E8E3BC-BAAE-44DE-99C2-7E67116E2BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4918535-C4E4-48EA-8619-1F6E01EEE2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +461,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -564,6 +570,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1785,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D395" sqref="D395"/>
+    <sheetView tabSelected="1" topLeftCell="A365" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G387" sqref="G387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5731,7 +5738,7 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400" s="4"/>
-      <c r="B400" s="14">
+      <c r="B400" s="26">
         <f>SUM(B397:B399)</f>
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
improve first person controller script
</commit_message>
<xml_diff>
--- a/documents/TimeRecord.xlsx
+++ b/documents/TimeRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\youre-not-alone\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F86A4BE-73BE-4F6F-8A6B-CCCFA46E6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F82E45-3940-4519-9CF5-94B02013F99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1901,7 +1901,7 @@
   <dimension ref="A1:F438"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A407" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E432" sqref="E432"/>
+      <selection activeCell="B436" sqref="B436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6252,8 +6252,8 @@
         <v>5</v>
       </c>
       <c r="B435" s="21">
-        <f>C411+C414+C418+C423+C425+C431</f>
-        <v>15</v>
+        <f>C411+C414+C418+C423+C425+C431+C429</f>
+        <v>17</v>
       </c>
       <c r="C435" s="21"/>
       <c r="D435" s="19"/>
@@ -6287,7 +6287,7 @@
       <c r="A438" s="4"/>
       <c r="B438" s="26">
         <f>SUM(B435:B437)</f>
-        <v>51.5</v>
+        <v>53.5</v>
       </c>
       <c r="C438" s="14"/>
       <c r="D438" s="14"/>

</xml_diff>